<commit_message>
V3: Add test results and update master file
</commit_message>
<xml_diff>
--- a/kpi-dashboard/Maturity-Framework-KPI-loveable.xlsx
+++ b/kpi-dashboard/Maturity-Framework-KPI-loveable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manojgupta/kpi-dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F69D1C0-18ED-504D-ADAE-5C12A687E767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7287A85D-2FF3-974C-BB05-8311E41C3698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29460" yWindow="500" windowWidth="28040" windowHeight="16420" activeTab="5" xr2:uid="{156CD2C2-A08D-D345-B6AF-813C3AC943F2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16560" activeTab="1" xr2:uid="{156CD2C2-A08D-D345-B6AF-813C3AC943F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Health Score Components" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Relationship Strength KPI" sheetId="6" r:id="rId6"/>
     <sheet name="Overall Health Score" sheetId="9" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -604,12 +604,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -619,6 +613,12 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -955,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B9C55D-0647-9B49-B65E-9419C99EE001}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,10 +986,10 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="14">
         <v>0.3</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -997,24 +997,24 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
+      <c r="A5" s="13"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="14">
         <v>0.2</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1022,24 +1022,24 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="14">
         <v>0.2</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1047,24 +1047,24 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="14">
         <v>0.15</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1072,26 +1072,26 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="14">
         <v>0.15</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
+    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="3" t="s">
         <v>91</v>
       </c>
@@ -1108,14 +1108,14 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="11"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1138,14 +1138,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DC42C4-EE8E-EC4E-8A0D-4C5926CD7D31}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:E25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="13"/>
+    <col min="3" max="3" width="10.83203125" style="11"/>
     <col min="4" max="4" width="15.6640625" customWidth="1"/>
     <col min="5" max="5" width="40.83203125" customWidth="1"/>
     <col min="7" max="7" width="35.1640625" customWidth="1"/>
@@ -1166,7 +1166,7 @@
       <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>126</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1189,7 +1189,7 @@
       <c r="B4" s="7">
         <v>0.3</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="11">
         <v>9</v>
       </c>
       <c r="D4" t="s">
@@ -1212,7 +1212,7 @@
       <c r="B5" s="7">
         <v>0.3</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="11">
         <v>9</v>
       </c>
       <c r="D5" t="s">
@@ -1235,7 +1235,7 @@
       <c r="B6" s="7">
         <v>0.3</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="11">
         <v>9</v>
       </c>
       <c r="D6" t="s">
@@ -1258,7 +1258,7 @@
       <c r="B7" s="7">
         <v>0.3</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="11">
         <v>9</v>
       </c>
       <c r="D7" t="s">
@@ -1281,7 +1281,7 @@
       <c r="B8" s="7">
         <v>0.3</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="11">
         <v>5</v>
       </c>
       <c r="D8" t="s">
@@ -1304,7 +1304,7 @@
       <c r="B9" s="7">
         <v>0.3</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="11">
         <v>8</v>
       </c>
       <c r="D9" t="s">
@@ -1327,7 +1327,7 @@
       <c r="B10" s="7">
         <v>0.3</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="11">
         <v>8</v>
       </c>
       <c r="D10" t="s">
@@ -1350,7 +1350,7 @@
       <c r="B11" s="7">
         <v>0.3</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="11">
         <v>6</v>
       </c>
       <c r="D11" t="s">
@@ -1373,7 +1373,7 @@
       <c r="B12" s="7">
         <v>0.3</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="11">
         <v>5</v>
       </c>
       <c r="D12" t="s">
@@ -1396,7 +1396,7 @@
       <c r="B13" s="7">
         <v>0.3</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>5</v>
       </c>
       <c r="D13" t="s">
@@ -1419,7 +1419,7 @@
       <c r="B14" s="7">
         <v>0.3</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="11">
         <v>9</v>
       </c>
       <c r="D14" t="s">
@@ -1442,7 +1442,7 @@
       <c r="B15" s="7">
         <v>0.3</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="11">
         <v>6</v>
       </c>
       <c r="D15" t="s">
@@ -1465,7 +1465,7 @@
       <c r="B16" s="7">
         <v>0.3</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="11">
         <v>6</v>
       </c>
       <c r="D16" t="s">
@@ -1488,7 +1488,7 @@
       <c r="B17" s="7">
         <v>0.3</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="11">
         <v>6</v>
       </c>
       <c r="D17" t="s">
@@ -1528,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F02D9C-9A8E-464C-80D4-9DC431C86131}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:E21"/>
+    <sheetView zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2000,7 +2000,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="A26:E31"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2464,7 +2464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF353381-CEA8-BF42-B8CA-D25DB9F02289}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="A15:E20"/>
     </sheetView>
   </sheetViews>
@@ -2741,7 +2741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9311BEF2-98FC-6E48-ACB3-50409BC0A2AA}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="183" zoomScaleNormal="189" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2781,7 +2781,7 @@
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="10" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2795,7 +2795,7 @@
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2809,7 +2809,7 @@
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="10" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>